<commit_message>
updates 12s code to remedy issue where replicate 124 was not being removed
</commit_message>
<xml_diff>
--- a/Deliverables/12S/regions/sbering/ADFG_12s_sbering_speciesxsamples.xlsx
+++ b/Deliverables/12S/regions/sbering/ADFG_12s_sbering_speciesxsamples.xlsx
@@ -1,186 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/Deliverables/12S/regions/sbering/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_5938EDF4C26E9381F6A65AC26B7DF75EAB4BE846" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2821C646-AED3-44AD-813C-932C36E6EDA1}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="absolute_abundance" sheetId="1" r:id="rId1"/>
     <sheet name="proportional_abundance" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
-  <si>
-    <t>LabID</t>
-  </si>
-  <si>
-    <t>Specimen.ID</t>
-  </si>
-  <si>
-    <t>Eleginus gracilis</t>
-  </si>
-  <si>
-    <t>Clupea pallasii</t>
-  </si>
-  <si>
-    <t>Osmerus mordax</t>
-  </si>
-  <si>
-    <t>Pungitius pungitius</t>
-  </si>
-  <si>
-    <t>Hypomesus olidus</t>
-  </si>
-  <si>
-    <t>Ammodytes hexapterus</t>
-  </si>
-  <si>
-    <t>Myoxocephalus spp.</t>
-  </si>
-  <si>
-    <t>Boreogadus saida</t>
-  </si>
-  <si>
-    <t>Lepidopsetta spp.</t>
-  </si>
-  <si>
-    <t>Eurymen gyrinus</t>
-  </si>
-  <si>
-    <t>Coregonus spp.</t>
-  </si>
-  <si>
-    <t>WADE-003-025</t>
-  </si>
-  <si>
-    <t>DL17HB001</t>
-  </si>
-  <si>
-    <t>WADE-003-026</t>
-  </si>
-  <si>
-    <t>DL17OME001</t>
-  </si>
-  <si>
-    <t>WADE-003-027</t>
-  </si>
-  <si>
-    <t>DL18OME001</t>
-  </si>
-  <si>
-    <t>WADE-003-028</t>
-  </si>
-  <si>
-    <t>DL18OME002</t>
-  </si>
-  <si>
-    <t>WADE-003-029</t>
-  </si>
-  <si>
-    <t>DL18OME003</t>
-  </si>
-  <si>
-    <t>WADE-003-030</t>
-  </si>
-  <si>
-    <t>DL18OME004</t>
-  </si>
-  <si>
-    <t>WADE-003-031</t>
-  </si>
-  <si>
-    <t>DL20OME001</t>
-  </si>
-  <si>
-    <t>WADE-003-032</t>
-  </si>
-  <si>
-    <t>DL20OME002</t>
-  </si>
-  <si>
-    <t>WADE-003-033</t>
-  </si>
-  <si>
-    <t>DL20OME003</t>
-  </si>
-  <si>
-    <t>WADE-003-035</t>
-  </si>
-  <si>
-    <t>DL22OME001</t>
-  </si>
-  <si>
-    <t>WADE-003-036</t>
-  </si>
-  <si>
-    <t>DL22OME002</t>
-  </si>
-  <si>
-    <t>WADE-003-037</t>
-  </si>
-  <si>
-    <t>DL22OME003</t>
-  </si>
-  <si>
-    <t>WADE-003-038</t>
-  </si>
-  <si>
-    <t>DL22OME004</t>
-  </si>
-  <si>
-    <t>WADE-003-039</t>
-  </si>
-  <si>
-    <t>DL22OME005</t>
-  </si>
-  <si>
-    <t>WADE-003-041</t>
-  </si>
-  <si>
-    <t>DL22SCM001</t>
-  </si>
-  <si>
-    <t>WADE-003-042</t>
-  </si>
-  <si>
-    <t>DL23OME001</t>
-  </si>
-  <si>
-    <t>WADE-003-043</t>
-  </si>
-  <si>
-    <t>DL23OME002</t>
-  </si>
-  <si>
-    <t>WADE-003-044</t>
-  </si>
-  <si>
-    <t>DL23OME003</t>
-  </si>
-  <si>
-    <t>WADE-003-045</t>
-  </si>
-  <si>
-    <t>DL23SCM001</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,21 +64,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -280,7 +108,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -314,7 +142,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -349,10 +176,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -525,67 +351,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LabID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Specimen.ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Eleginus gracilis</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Clupea pallasii</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Osmerus mordax</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Pungitius pungitius</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Hypomesus olidus</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Ammodytes hexapterus</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Myoxocephalus spp.</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Boreogadus saida</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Lepidopsetta spp.</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Eurymen gyrinus</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Coregonus spp.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>WADE-003-025</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DL17HB001</t>
+        </is>
       </c>
       <c r="C2">
         <v>20531</v>
@@ -621,12 +470,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>WADE-003-026</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>DL17OME001</t>
+        </is>
       </c>
       <c r="C3">
         <v>35542</v>
@@ -662,12 +515,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>WADE-003-027</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DL18OME001</t>
+        </is>
       </c>
       <c r="C4">
         <v>26316</v>
@@ -703,12 +560,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WADE-003-028</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DL18OME002</t>
+        </is>
       </c>
       <c r="C5">
         <v>1515</v>
@@ -744,12 +605,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>WADE-003-029</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DL18OME003</t>
+        </is>
       </c>
       <c r="C6">
         <v>10979</v>
@@ -785,12 +650,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WADE-003-030</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DL18OME004</t>
+        </is>
       </c>
       <c r="C7">
         <v>1479</v>
@@ -826,12 +695,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WADE-003-031</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DL20OME001</t>
+        </is>
       </c>
       <c r="C8">
         <v>49244</v>
@@ -867,12 +740,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>WADE-003-032</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DL20OME002</t>
+        </is>
       </c>
       <c r="C9">
         <v>586</v>
@@ -908,12 +785,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WADE-003-033</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DL20OME003</t>
+        </is>
       </c>
       <c r="C10">
         <v>21653</v>
@@ -949,12 +830,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WADE-003-035</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DL22OME001</t>
+        </is>
       </c>
       <c r="C11">
         <v>8427</v>
@@ -990,12 +875,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WADE-003-036</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DL22OME002</t>
+        </is>
       </c>
       <c r="C12">
         <v>8127</v>
@@ -1031,12 +920,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WADE-003-037</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DL22OME003</t>
+        </is>
       </c>
       <c r="C13">
         <v>14299</v>
@@ -1072,12 +965,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WADE-003-038</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DL22OME004</t>
+        </is>
       </c>
       <c r="C14">
         <v>6509</v>
@@ -1113,12 +1010,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WADE-003-039</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DL22OME005</t>
+        </is>
       </c>
       <c r="C15">
         <v>18604</v>
@@ -1154,12 +1055,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WADE-003-041</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DL22SCM001</t>
+        </is>
       </c>
       <c r="C16">
         <v>546915</v>
@@ -1195,12 +1100,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>WADE-003-042</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DL23OME001</t>
+        </is>
       </c>
       <c r="C17">
         <v>30625</v>
@@ -1236,12 +1145,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WADE-003-043</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DL23OME002</t>
+        </is>
       </c>
       <c r="C18">
         <v>11413</v>
@@ -1277,12 +1190,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>WADE-003-044</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DL23OME003</t>
+        </is>
       </c>
       <c r="C19">
         <v>97</v>
@@ -1318,12 +1235,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>WADE-003-045</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DL23SCM001</t>
+        </is>
       </c>
       <c r="C20">
         <v>3189</v>
@@ -1365,80 +1286,105 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LabID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Specimen.ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Eleginus gracilis</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Clupea pallasii</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Osmerus mordax</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Pungitius pungitius</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Hypomesus olidus</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Ammodytes hexapterus</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Myoxocephalus spp.</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Boreogadus saida</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Lepidopsetta spp.</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Eurymen gyrinus</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Coregonus spp.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>WADE-003-025</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DL17HB001</t>
+        </is>
       </c>
       <c r="C2">
-        <v>0.50646000000000002</v>
+        <v>0.50646</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.49187999999999998</v>
+        <v>0.49188</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1.65E-3</v>
+        <v>0.00165</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1459,21 +1405,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>WADE-003-026</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>DL17OME001</t>
+        </is>
       </c>
       <c r="C3">
-        <v>0.97662000000000004</v>
+        <v>0.97662</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>7.7999999999999996E-3</v>
+        <v>0.0078</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1485,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1.558E-2</v>
+        <v>0.01558</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1500,15 +1450,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>WADE-003-027</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DL18OME001</t>
+        </is>
       </c>
       <c r="C4">
-        <v>0.99882000000000004</v>
+        <v>0.99882</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1523,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1.1800000000000001E-3</v>
+        <v>0.00118</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1541,21 +1495,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WADE-003-028</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DL18OME002</t>
+        </is>
       </c>
       <c r="C5">
-        <v>0.98248999999999997</v>
+        <v>0.98249</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>2.5899999999999999E-3</v>
+        <v>0.00259</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1564,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1.4919999999999999E-2</v>
+        <v>0.01492</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1582,12 +1540,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>WADE-003-029</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DL18OME003</t>
+        </is>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1623,12 +1585,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WADE-003-030</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DL18OME004</t>
+        </is>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1664,12 +1630,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WADE-003-031</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DL20OME001</t>
+        </is>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1705,12 +1675,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>WADE-003-032</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DL20OME002</t>
+        </is>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1746,21 +1720,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WADE-003-033</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DL20OME003</t>
+        </is>
       </c>
       <c r="C10">
-        <v>0.98185999999999996</v>
+        <v>0.98186</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1.814E-2</v>
+        <v>0.01814</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1787,15 +1765,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WADE-003-035</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DL22OME001</t>
+        </is>
       </c>
       <c r="C11">
-        <v>0.99975999999999998</v>
+        <v>0.99976</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1804,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>2.4000000000000001E-4</v>
+        <v>0.00024</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1828,21 +1810,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WADE-003-036</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DL22OME002</t>
+        </is>
       </c>
       <c r="C12">
-        <v>0.99975000000000003</v>
+        <v>0.99975</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>2.5000000000000001E-4</v>
+        <v>0.00025</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1869,21 +1855,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WADE-003-037</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DL22OME003</t>
+        </is>
       </c>
       <c r="C13">
-        <v>0.92520000000000002</v>
+        <v>0.9252</v>
       </c>
       <c r="D13">
-        <v>3.49E-3</v>
+        <v>0.00349</v>
       </c>
       <c r="E13">
-        <v>6.7159999999999997E-2</v>
+        <v>0.06716</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1892,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>4.1399999999999996E-3</v>
+        <v>0.00414</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1910,21 +1900,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WADE-003-038</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DL22OME004</t>
+        </is>
       </c>
       <c r="C14">
-        <v>0.57908999999999999</v>
+        <v>0.57909</v>
       </c>
       <c r="D14">
         <v>0.36495</v>
       </c>
       <c r="E14">
-        <v>4.2700000000000004E-3</v>
+        <v>0.00427</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1939,24 +1933,28 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1.77E-2</v>
+        <v>0.0177</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>3.3989999999999999E-2</v>
+        <v>0.03399</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WADE-003-039</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DL22OME005</t>
+        </is>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1992,27 +1990,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WADE-003-041</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DL22SCM001</t>
+        </is>
       </c>
       <c r="C16">
         <v>0.39476</v>
       </c>
       <c r="D16">
-        <v>1.9000000000000001E-4</v>
+        <v>0.00019</v>
       </c>
       <c r="E16">
-        <v>0.50960000000000005</v>
+        <v>0.5096000000000001</v>
       </c>
       <c r="F16">
-        <v>6.8629999999999997E-2</v>
+        <v>0.06863</v>
       </c>
       <c r="G16">
-        <v>2.682E-2</v>
+        <v>0.02682</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2033,21 +2035,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>WADE-003-042</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DL23OME001</t>
+        </is>
       </c>
       <c r="C17">
-        <v>0.98619000000000001</v>
+        <v>0.98619</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1.269E-2</v>
+        <v>0.01269</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -2056,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>1.1299999999999999E-3</v>
+        <v>0.00113</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2074,15 +2080,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WADE-003-043</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DL23OME002</t>
+        </is>
       </c>
       <c r="C18">
-        <v>0.87082000000000004</v>
+        <v>0.87082</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2097,7 +2107,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.12917999999999999</v>
+        <v>0.12918</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -2115,21 +2125,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>WADE-003-044</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DL23OME003</t>
+        </is>
       </c>
       <c r="C19">
-        <v>4.2540000000000001E-2</v>
+        <v>0.04254</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>2.8070000000000001E-2</v>
+        <v>0.02807</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2138,16 +2152,16 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>4.8199999999999996E-3</v>
+        <v>0.00482</v>
       </c>
       <c r="I19">
-        <v>0.90351000000000004</v>
+        <v>0.90351</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
-        <v>2.1049999999999999E-2</v>
+        <v>0.02105</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2156,21 +2170,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>WADE-003-045</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DL23SCM001</t>
+        </is>
       </c>
       <c r="C20">
-        <v>0.71453999999999995</v>
+        <v>0.71454</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>2.9350000000000001E-2</v>
+        <v>0.02935</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2194,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>4.616E-2</v>
+        <v>0.04616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>